<commit_message>
Updated README and 3-way partition method
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -470,19 +470,19 @@
         <v>50000</v>
       </c>
       <c r="B2" t="n">
-        <v>10.3</v>
+        <v>3.8</v>
       </c>
       <c r="C2" t="n">
-        <v>10.25</v>
+        <v>2.4</v>
       </c>
       <c r="D2" t="n">
-        <v>5.1</v>
+        <v>5.5</v>
       </c>
       <c r="E2" t="n">
-        <v>38.8</v>
+        <v>42.5</v>
       </c>
       <c r="F2" t="n">
-        <v>26.15</v>
+        <v>28.15</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>100000</v>
       </c>
       <c r="B3" t="n">
-        <v>22.3</v>
+        <v>7.45</v>
       </c>
       <c r="C3" t="n">
-        <v>22.1</v>
+        <v>4.95</v>
       </c>
       <c r="D3" t="n">
-        <v>10.9</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>79.7</v>
+        <v>87.55</v>
       </c>
       <c r="F3" t="n">
-        <v>55.2</v>
+        <v>59.55</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>150000</v>
       </c>
       <c r="B4" t="n">
-        <v>34.8</v>
+        <v>11.45</v>
       </c>
       <c r="C4" t="n">
-        <v>34.75</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>17.55</v>
+        <v>19.25</v>
       </c>
       <c r="E4" t="n">
-        <v>122.35</v>
+        <v>137.5</v>
       </c>
       <c r="F4" t="n">
-        <v>85.7</v>
+        <v>92.3</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>200000</v>
       </c>
       <c r="B5" t="n">
-        <v>47.95</v>
+        <v>15.85</v>
       </c>
       <c r="C5" t="n">
-        <v>48.2</v>
+        <v>10.35</v>
       </c>
       <c r="D5" t="n">
-        <v>22.9</v>
+        <v>25.1</v>
       </c>
       <c r="E5" t="n">
-        <v>163.55</v>
+        <v>180.75</v>
       </c>
       <c r="F5" t="n">
-        <v>117.2</v>
+        <v>126.3</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>250000</v>
       </c>
       <c r="B6" t="n">
-        <v>60.85</v>
+        <v>19.9</v>
       </c>
       <c r="C6" t="n">
-        <v>61.7</v>
+        <v>14.95</v>
       </c>
       <c r="D6" t="n">
-        <v>28</v>
+        <v>30.5</v>
       </c>
       <c r="E6" t="n">
-        <v>197.35</v>
+        <v>221.7</v>
       </c>
       <c r="F6" t="n">
-        <v>148.25</v>
+        <v>162.2</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>300000</v>
       </c>
       <c r="B7" t="n">
-        <v>74.09999999999999</v>
+        <v>23.4</v>
       </c>
       <c r="C7" t="n">
-        <v>74.59999999999999</v>
+        <v>18.45</v>
       </c>
       <c r="D7" t="n">
-        <v>36.55</v>
+        <v>40.7</v>
       </c>
       <c r="E7" t="n">
-        <v>248.85</v>
+        <v>280.25</v>
       </c>
       <c r="F7" t="n">
-        <v>180.1</v>
+        <v>196.1</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>350000</v>
       </c>
       <c r="B8" t="n">
-        <v>86.7</v>
+        <v>27.8</v>
       </c>
       <c r="C8" t="n">
-        <v>88.2</v>
+        <v>20.4</v>
       </c>
       <c r="D8" t="n">
-        <v>42.1</v>
+        <v>45.6</v>
       </c>
       <c r="E8" t="n">
-        <v>291.5</v>
+        <v>326.7</v>
       </c>
       <c r="F8" t="n">
-        <v>212.55</v>
+        <v>231.65</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>400000</v>
       </c>
       <c r="B9" t="n">
-        <v>101.6</v>
+        <v>33</v>
       </c>
       <c r="C9" t="n">
-        <v>102.95</v>
+        <v>23.05</v>
       </c>
       <c r="D9" t="n">
-        <v>47.9</v>
+        <v>52.6</v>
       </c>
       <c r="E9" t="n">
-        <v>330.95</v>
+        <v>367.9</v>
       </c>
       <c r="F9" t="n">
-        <v>245.15</v>
+        <v>264.9</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>450000</v>
       </c>
       <c r="B10" t="n">
-        <v>113.95</v>
+        <v>35.55</v>
       </c>
       <c r="C10" t="n">
-        <v>115.75</v>
+        <v>25.25</v>
       </c>
       <c r="D10" t="n">
-        <v>53.5</v>
+        <v>57.9</v>
       </c>
       <c r="E10" t="n">
-        <v>367.45</v>
+        <v>410.25</v>
       </c>
       <c r="F10" t="n">
-        <v>278.75</v>
+        <v>302.65</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>500000</v>
       </c>
       <c r="B11" t="n">
-        <v>130.1</v>
+        <v>39.3</v>
       </c>
       <c r="C11" t="n">
-        <v>133.7</v>
+        <v>31.5</v>
       </c>
       <c r="D11" t="n">
-        <v>59</v>
+        <v>63.75</v>
       </c>
       <c r="E11" t="n">
-        <v>403.15</v>
+        <v>448.9</v>
       </c>
       <c r="F11" t="n">
-        <v>311.8</v>
+        <v>339.75</v>
       </c>
     </row>
     <row r="12">
@@ -670,19 +670,19 @@
         <v>550000</v>
       </c>
       <c r="B12" t="n">
-        <v>143.2</v>
+        <v>43.4</v>
       </c>
       <c r="C12" t="n">
-        <v>144.05</v>
+        <v>34.55</v>
       </c>
       <c r="D12" t="n">
-        <v>69</v>
+        <v>76.05</v>
       </c>
       <c r="E12" t="n">
-        <v>456.75</v>
+        <v>509.25</v>
       </c>
       <c r="F12" t="n">
-        <v>345.55</v>
+        <v>374.7</v>
       </c>
     </row>
     <row r="13">
@@ -690,19 +690,19 @@
         <v>600000</v>
       </c>
       <c r="B13" t="n">
-        <v>158</v>
+        <v>48.3</v>
       </c>
       <c r="C13" t="n">
-        <v>160</v>
+        <v>37.15</v>
       </c>
       <c r="D13" t="n">
-        <v>76.09999999999999</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>508.5</v>
+        <v>561.9</v>
       </c>
       <c r="F13" t="n">
-        <v>379.55</v>
+        <v>407.75</v>
       </c>
     </row>
     <row r="14">
@@ -710,19 +710,19 @@
         <v>650000</v>
       </c>
       <c r="B14" t="n">
-        <v>171.25</v>
+        <v>52.6</v>
       </c>
       <c r="C14" t="n">
-        <v>174.6</v>
+        <v>39</v>
       </c>
       <c r="D14" t="n">
-        <v>81.75</v>
+        <v>90.2</v>
       </c>
       <c r="E14" t="n">
-        <v>553.05</v>
+        <v>614.1</v>
       </c>
       <c r="F14" t="n">
-        <v>413.85</v>
+        <v>445.25</v>
       </c>
     </row>
     <row r="15">
@@ -730,19 +730,19 @@
         <v>700000</v>
       </c>
       <c r="B15" t="n">
-        <v>185.7</v>
+        <v>57.45</v>
       </c>
       <c r="C15" t="n">
-        <v>190.25</v>
+        <v>42.2</v>
       </c>
       <c r="D15" t="n">
-        <v>87.84999999999999</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>594.95</v>
+        <v>660.55</v>
       </c>
       <c r="F15" t="n">
-        <v>448.25</v>
+        <v>482.2</v>
       </c>
     </row>
     <row r="16">
@@ -750,19 +750,19 @@
         <v>750000</v>
       </c>
       <c r="B16" t="n">
-        <v>199.25</v>
+        <v>63.9</v>
       </c>
       <c r="C16" t="n">
-        <v>203.25</v>
+        <v>44.95</v>
       </c>
       <c r="D16" t="n">
-        <v>93.2</v>
+        <v>100.9</v>
       </c>
       <c r="E16" t="n">
-        <v>635.9</v>
+        <v>705.05</v>
       </c>
       <c r="F16" t="n">
-        <v>482.6</v>
+        <v>520.15</v>
       </c>
     </row>
     <row r="17">
@@ -770,19 +770,19 @@
         <v>800000</v>
       </c>
       <c r="B17" t="n">
-        <v>216.15</v>
+        <v>66.8</v>
       </c>
       <c r="C17" t="n">
-        <v>221.45</v>
+        <v>47.5</v>
       </c>
       <c r="D17" t="n">
-        <v>99.55</v>
+        <v>109.3</v>
       </c>
       <c r="E17" t="n">
-        <v>675.5</v>
+        <v>749.2</v>
       </c>
       <c r="F17" t="n">
-        <v>516.95</v>
+        <v>558.2</v>
       </c>
     </row>
     <row r="18">
@@ -790,19 +790,19 @@
         <v>850000</v>
       </c>
       <c r="B18" t="n">
-        <v>229.75</v>
+        <v>70.8</v>
       </c>
       <c r="C18" t="n">
-        <v>234.45</v>
+        <v>51</v>
       </c>
       <c r="D18" t="n">
-        <v>105.2</v>
+        <v>115</v>
       </c>
       <c r="E18" t="n">
-        <v>713.9</v>
+        <v>792.05</v>
       </c>
       <c r="F18" t="n">
-        <v>552.1</v>
+        <v>596.35</v>
       </c>
     </row>
     <row r="19">
@@ -810,19 +810,19 @@
         <v>900000</v>
       </c>
       <c r="B19" t="n">
-        <v>242.9</v>
+        <v>73.2</v>
       </c>
       <c r="C19" t="n">
-        <v>248.95</v>
+        <v>52.15</v>
       </c>
       <c r="D19" t="n">
-        <v>111.05</v>
+        <v>120.6</v>
       </c>
       <c r="E19" t="n">
-        <v>749.8</v>
+        <v>827.45</v>
       </c>
       <c r="F19" t="n">
-        <v>587.1</v>
+        <v>629.25</v>
       </c>
     </row>
     <row r="20">
@@ -830,19 +830,19 @@
         <v>950000</v>
       </c>
       <c r="B20" t="n">
-        <v>258.15</v>
+        <v>76.25</v>
       </c>
       <c r="C20" t="n">
-        <v>266.95</v>
+        <v>58.65</v>
       </c>
       <c r="D20" t="n">
-        <v>117</v>
+        <v>127.4</v>
       </c>
       <c r="E20" t="n">
-        <v>787.75</v>
+        <v>869.7</v>
       </c>
       <c r="F20" t="n">
-        <v>622.25</v>
+        <v>669.6</v>
       </c>
     </row>
     <row r="21">
@@ -850,19 +850,19 @@
         <v>1000000</v>
       </c>
       <c r="B21" t="n">
-        <v>276.95</v>
+        <v>78.2</v>
       </c>
       <c r="C21" t="n">
-        <v>289.05</v>
+        <v>64.34999999999999</v>
       </c>
       <c r="D21" t="n">
-        <v>122.9</v>
+        <v>134.1</v>
       </c>
       <c r="E21" t="n">
-        <v>823.55</v>
+        <v>913.55</v>
       </c>
       <c r="F21" t="n">
-        <v>656.9</v>
+        <v>708.9</v>
       </c>
     </row>
     <row r="22">
@@ -870,19 +870,19 @@
         <v>1050000</v>
       </c>
       <c r="B22" t="n">
-        <v>290.55</v>
+        <v>80.95</v>
       </c>
       <c r="C22" t="n">
-        <v>293.5</v>
+        <v>68.25</v>
       </c>
       <c r="D22" t="n">
-        <v>129.05</v>
+        <v>140.35</v>
       </c>
       <c r="E22" t="n">
-        <v>865.9</v>
+        <v>960.75</v>
       </c>
       <c r="F22" t="n">
-        <v>692.5</v>
+        <v>742.95</v>
       </c>
     </row>
     <row r="23">
@@ -890,19 +890,19 @@
         <v>1100000</v>
       </c>
       <c r="B23" t="n">
-        <v>306.2</v>
+        <v>88.7</v>
       </c>
       <c r="C23" t="n">
-        <v>310.1</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>144.3</v>
+        <v>156.05</v>
       </c>
       <c r="E23" t="n">
-        <v>932.95</v>
+        <v>1033.25</v>
       </c>
       <c r="F23" t="n">
-        <v>728.5</v>
+        <v>782.6</v>
       </c>
     </row>
     <row r="24">
@@ -910,19 +910,19 @@
         <v>1150000</v>
       </c>
       <c r="B24" t="n">
-        <v>319.05</v>
+        <v>95.2</v>
       </c>
       <c r="C24" t="n">
-        <v>326.15</v>
+        <v>74.25</v>
       </c>
       <c r="D24" t="n">
-        <v>152.75</v>
+        <v>169.3</v>
       </c>
       <c r="E24" t="n">
-        <v>987.7</v>
+        <v>1108.45</v>
       </c>
       <c r="F24" t="n">
-        <v>763.55</v>
+        <v>826.9</v>
       </c>
     </row>
     <row r="25">
@@ -930,19 +930,19 @@
         <v>1200000</v>
       </c>
       <c r="B25" t="n">
-        <v>335.7</v>
+        <v>100.05</v>
       </c>
       <c r="C25" t="n">
-        <v>342.4</v>
+        <v>78.25</v>
       </c>
       <c r="D25" t="n">
-        <v>159</v>
+        <v>178.6</v>
       </c>
       <c r="E25" t="n">
-        <v>1038</v>
+        <v>1177.75</v>
       </c>
       <c r="F25" t="n">
-        <v>798.75</v>
+        <v>873.2</v>
       </c>
     </row>
     <row r="26">
@@ -950,19 +950,19 @@
         <v>1250000</v>
       </c>
       <c r="B26" t="n">
-        <v>347.8</v>
+        <v>102.5</v>
       </c>
       <c r="C26" t="n">
-        <v>356.05</v>
+        <v>79.05</v>
       </c>
       <c r="D26" t="n">
-        <v>165</v>
+        <v>179.4</v>
       </c>
       <c r="E26" t="n">
-        <v>1083.15</v>
+        <v>1191.45</v>
       </c>
       <c r="F26" t="n">
-        <v>834.2</v>
+        <v>891.9</v>
       </c>
     </row>
     <row r="27">
@@ -970,19 +970,19 @@
         <v>1300000</v>
       </c>
       <c r="B27" t="n">
-        <v>365</v>
+        <v>107.7</v>
       </c>
       <c r="C27" t="n">
-        <v>374.95</v>
+        <v>80.75</v>
       </c>
       <c r="D27" t="n">
-        <v>171.15</v>
+        <v>188.7</v>
       </c>
       <c r="E27" t="n">
-        <v>1129.05</v>
+        <v>1250.1</v>
       </c>
       <c r="F27" t="n">
-        <v>870.45</v>
+        <v>934.4</v>
       </c>
     </row>
     <row r="28">
@@ -990,19 +990,19 @@
         <v>1350000</v>
       </c>
       <c r="B28" t="n">
-        <v>377.1</v>
+        <v>114.9</v>
       </c>
       <c r="C28" t="n">
-        <v>388.75</v>
+        <v>83.65000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>177.5</v>
+        <v>193.4</v>
       </c>
       <c r="E28" t="n">
-        <v>1172.75</v>
+        <v>1293.1</v>
       </c>
       <c r="F28" t="n">
-        <v>905.75</v>
+        <v>975.35</v>
       </c>
     </row>
     <row r="29">
@@ -1010,19 +1010,19 @@
         <v>1400000</v>
       </c>
       <c r="B29" t="n">
-        <v>394.75</v>
+        <v>119.95</v>
       </c>
       <c r="C29" t="n">
-        <v>409</v>
+        <v>87.55</v>
       </c>
       <c r="D29" t="n">
-        <v>183.45</v>
+        <v>199.95</v>
       </c>
       <c r="E29" t="n">
-        <v>1214.35</v>
+        <v>1348.1</v>
       </c>
       <c r="F29" t="n">
-        <v>942.05</v>
+        <v>1014.2</v>
       </c>
     </row>
     <row r="30">
@@ -1030,19 +1030,19 @@
         <v>1450000</v>
       </c>
       <c r="B30" t="n">
-        <v>415.4</v>
+        <v>122.7</v>
       </c>
       <c r="C30" t="n">
-        <v>438.7</v>
+        <v>89.34999999999999</v>
       </c>
       <c r="D30" t="n">
-        <v>189.7</v>
+        <v>205.3</v>
       </c>
       <c r="E30" t="n">
-        <v>1256.15</v>
+        <v>1389.55</v>
       </c>
       <c r="F30" t="n">
-        <v>978.3</v>
+        <v>1047.3</v>
       </c>
     </row>
     <row r="31">
@@ -1050,19 +1050,19 @@
         <v>1500000</v>
       </c>
       <c r="B31" t="n">
-        <v>431.7</v>
+        <v>129.1</v>
       </c>
       <c r="C31" t="n">
-        <v>443.25</v>
+        <v>92.45</v>
       </c>
       <c r="D31" t="n">
-        <v>198.8</v>
+        <v>211.6</v>
       </c>
       <c r="E31" t="n">
-        <v>1317.3</v>
+        <v>1432.8</v>
       </c>
       <c r="F31" t="n">
-        <v>1029.65</v>
+        <v>1085.2</v>
       </c>
     </row>
     <row r="32">
@@ -1070,19 +1070,19 @@
         <v>1550000</v>
       </c>
       <c r="B32" t="n">
-        <v>436.2</v>
+        <v>133.15</v>
       </c>
       <c r="C32" t="n">
-        <v>447.45</v>
+        <v>96.05</v>
       </c>
       <c r="D32" t="n">
-        <v>201.9</v>
+        <v>219.95</v>
       </c>
       <c r="E32" t="n">
-        <v>1338.95</v>
+        <v>1480.65</v>
       </c>
       <c r="F32" t="n">
-        <v>1050.5</v>
+        <v>1126.8</v>
       </c>
     </row>
     <row r="33">
@@ -1090,19 +1090,19 @@
         <v>1600000</v>
       </c>
       <c r="B33" t="n">
-        <v>459.55</v>
+        <v>138.15</v>
       </c>
       <c r="C33" t="n">
-        <v>476.1</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>208</v>
+        <v>225.75</v>
       </c>
       <c r="E33" t="n">
-        <v>1378.95</v>
+        <v>1519.5</v>
       </c>
       <c r="F33" t="n">
-        <v>1086.6</v>
+        <v>1161.1</v>
       </c>
     </row>
     <row r="34">
@@ -1110,19 +1110,19 @@
         <v>1650000</v>
       </c>
       <c r="B34" t="n">
-        <v>467.3</v>
+        <v>144</v>
       </c>
       <c r="C34" t="n">
-        <v>481.3</v>
+        <v>101.25</v>
       </c>
       <c r="D34" t="n">
-        <v>214.4</v>
+        <v>234.75</v>
       </c>
       <c r="E34" t="n">
-        <v>1418.25</v>
+        <v>1579.35</v>
       </c>
       <c r="F34" t="n">
-        <v>1123.65</v>
+        <v>1210.75</v>
       </c>
     </row>
     <row r="35">
@@ -1130,19 +1130,19 @@
         <v>1700000</v>
       </c>
       <c r="B35" t="n">
-        <v>488.35</v>
+        <v>145.15</v>
       </c>
       <c r="C35" t="n">
-        <v>505.2</v>
+        <v>103.4</v>
       </c>
       <c r="D35" t="n">
-        <v>220.3</v>
+        <v>239.55</v>
       </c>
       <c r="E35" t="n">
-        <v>1456.8</v>
+        <v>1610.75</v>
       </c>
       <c r="F35" t="n">
-        <v>1160.1</v>
+        <v>1243.8</v>
       </c>
     </row>
     <row r="36">
@@ -1150,19 +1150,19 @@
         <v>1750000</v>
       </c>
       <c r="B36" t="n">
-        <v>500</v>
+        <v>150.35</v>
       </c>
       <c r="C36" t="n">
-        <v>516.5</v>
+        <v>107.6</v>
       </c>
       <c r="D36" t="n">
-        <v>226.55</v>
+        <v>246.85</v>
       </c>
       <c r="E36" t="n">
-        <v>1494.25</v>
+        <v>1663.8</v>
       </c>
       <c r="F36" t="n">
-        <v>1196.7</v>
+        <v>1289.55</v>
       </c>
     </row>
     <row r="37">
@@ -1170,19 +1170,19 @@
         <v>1800000</v>
       </c>
       <c r="B37" t="n">
-        <v>517</v>
+        <v>151.55</v>
       </c>
       <c r="C37" t="n">
-        <v>538</v>
+        <v>109.85</v>
       </c>
       <c r="D37" t="n">
-        <v>232.5</v>
+        <v>254.25</v>
       </c>
       <c r="E37" t="n">
-        <v>1531.2</v>
+        <v>1697.3</v>
       </c>
       <c r="F37" t="n">
-        <v>1233.9</v>
+        <v>1326.3</v>
       </c>
     </row>
     <row r="38">
@@ -1190,19 +1190,19 @@
         <v>1850000</v>
       </c>
       <c r="B38" t="n">
-        <v>530.6</v>
+        <v>156.8</v>
       </c>
       <c r="C38" t="n">
-        <v>552.05</v>
+        <v>115.75</v>
       </c>
       <c r="D38" t="n">
-        <v>238.95</v>
+        <v>263.8</v>
       </c>
       <c r="E38" t="n">
-        <v>1570.1</v>
+        <v>1762.6</v>
       </c>
       <c r="F38" t="n">
-        <v>1271</v>
+        <v>1381.4</v>
       </c>
     </row>
     <row r="39">
@@ -1210,19 +1210,19 @@
         <v>1900000</v>
       </c>
       <c r="B39" t="n">
-        <v>549.45</v>
+        <v>161.6</v>
       </c>
       <c r="C39" t="n">
-        <v>575.9</v>
+        <v>126.75</v>
       </c>
       <c r="D39" t="n">
-        <v>244.95</v>
+        <v>275.85</v>
       </c>
       <c r="E39" t="n">
-        <v>1607.7</v>
+        <v>1818.6</v>
       </c>
       <c r="F39" t="n">
-        <v>1308.65</v>
+        <v>1434.15</v>
       </c>
     </row>
     <row r="40">
@@ -1230,19 +1230,19 @@
         <v>1950000</v>
       </c>
       <c r="B40" t="n">
-        <v>563.55</v>
+        <v>164.45</v>
       </c>
       <c r="C40" t="n">
-        <v>592.1</v>
+        <v>135</v>
       </c>
       <c r="D40" t="n">
-        <v>251.25</v>
+        <v>277.9</v>
       </c>
       <c r="E40" t="n">
-        <v>1644.1</v>
+        <v>1861.5</v>
       </c>
       <c r="F40" t="n">
-        <v>1345.9</v>
+        <v>1477.7</v>
       </c>
     </row>
     <row r="41">
@@ -1250,19 +1250,19 @@
         <v>2000000</v>
       </c>
       <c r="B41" t="n">
-        <v>587.5</v>
+        <v>167</v>
       </c>
       <c r="C41" t="n">
-        <v>622.4</v>
+        <v>140.05</v>
       </c>
       <c r="D41" t="n">
-        <v>257.4</v>
+        <v>287.25</v>
       </c>
       <c r="E41" t="n">
-        <v>1682.1</v>
+        <v>1907.3</v>
       </c>
       <c r="F41" t="n">
-        <v>1381.85</v>
+        <v>1514.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now outperforms std::sort in all 4 cases
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -470,19 +470,19 @@
         <v>50000</v>
       </c>
       <c r="B2" t="n">
-        <v>3.8</v>
+        <v>3.35</v>
       </c>
       <c r="C2" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="D2" t="n">
-        <v>5.5</v>
+        <v>7.4</v>
       </c>
       <c r="E2" t="n">
-        <v>42.5</v>
+        <v>42.25</v>
       </c>
       <c r="F2" t="n">
-        <v>28.15</v>
+        <v>26.75</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>100000</v>
       </c>
       <c r="B3" t="n">
-        <v>7.45</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>4.95</v>
+        <v>4.4</v>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>15.2</v>
       </c>
       <c r="E3" t="n">
-        <v>87.55</v>
+        <v>87.84999999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>59.55</v>
+        <v>57.05</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>150000</v>
       </c>
       <c r="B4" t="n">
-        <v>11.45</v>
+        <v>10.2</v>
       </c>
       <c r="C4" t="n">
-        <v>8.199999999999999</v>
+        <v>7.45</v>
       </c>
       <c r="D4" t="n">
-        <v>19.25</v>
+        <v>22.15</v>
       </c>
       <c r="E4" t="n">
-        <v>137.5</v>
+        <v>132.9</v>
       </c>
       <c r="F4" t="n">
-        <v>92.3</v>
+        <v>87.65000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>200000</v>
       </c>
       <c r="B5" t="n">
-        <v>15.85</v>
+        <v>14.2</v>
       </c>
       <c r="C5" t="n">
-        <v>10.35</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>25.1</v>
+        <v>31.35</v>
       </c>
       <c r="E5" t="n">
-        <v>180.75</v>
+        <v>176.1</v>
       </c>
       <c r="F5" t="n">
-        <v>126.3</v>
+        <v>119.05</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>250000</v>
       </c>
       <c r="B6" t="n">
-        <v>19.9</v>
+        <v>16.65</v>
       </c>
       <c r="C6" t="n">
-        <v>14.95</v>
+        <v>13.1</v>
       </c>
       <c r="D6" t="n">
-        <v>30.5</v>
+        <v>38.55</v>
       </c>
       <c r="E6" t="n">
-        <v>221.7</v>
+        <v>216.3</v>
       </c>
       <c r="F6" t="n">
-        <v>162.2</v>
+        <v>152.05</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>300000</v>
       </c>
       <c r="B7" t="n">
-        <v>23.4</v>
+        <v>21.5</v>
       </c>
       <c r="C7" t="n">
-        <v>18.45</v>
+        <v>14.8</v>
       </c>
       <c r="D7" t="n">
-        <v>40.7</v>
+        <v>48.4</v>
       </c>
       <c r="E7" t="n">
-        <v>280.25</v>
+        <v>273.25</v>
       </c>
       <c r="F7" t="n">
-        <v>196.1</v>
+        <v>186.15</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>350000</v>
       </c>
       <c r="B8" t="n">
-        <v>27.8</v>
+        <v>25.2</v>
       </c>
       <c r="C8" t="n">
-        <v>20.4</v>
+        <v>17.5</v>
       </c>
       <c r="D8" t="n">
-        <v>45.6</v>
+        <v>59.25</v>
       </c>
       <c r="E8" t="n">
-        <v>326.7</v>
+        <v>318.1</v>
       </c>
       <c r="F8" t="n">
-        <v>231.65</v>
+        <v>218.7</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>400000</v>
       </c>
       <c r="B9" t="n">
-        <v>33</v>
+        <v>29.05</v>
       </c>
       <c r="C9" t="n">
-        <v>23.05</v>
+        <v>19.75</v>
       </c>
       <c r="D9" t="n">
-        <v>52.6</v>
+        <v>66.2</v>
       </c>
       <c r="E9" t="n">
-        <v>367.9</v>
+        <v>360.55</v>
       </c>
       <c r="F9" t="n">
-        <v>264.9</v>
+        <v>253.6</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>450000</v>
       </c>
       <c r="B10" t="n">
-        <v>35.55</v>
+        <v>32.6</v>
       </c>
       <c r="C10" t="n">
-        <v>25.25</v>
+        <v>22.35</v>
       </c>
       <c r="D10" t="n">
-        <v>57.9</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>410.25</v>
+        <v>402.85</v>
       </c>
       <c r="F10" t="n">
-        <v>302.65</v>
+        <v>289.1</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>500000</v>
       </c>
       <c r="B11" t="n">
-        <v>39.3</v>
+        <v>35.15</v>
       </c>
       <c r="C11" t="n">
-        <v>31.5</v>
+        <v>27.35</v>
       </c>
       <c r="D11" t="n">
-        <v>63.75</v>
+        <v>81.7</v>
       </c>
       <c r="E11" t="n">
-        <v>448.9</v>
+        <v>441.8</v>
       </c>
       <c r="F11" t="n">
-        <v>339.75</v>
+        <v>320.75</v>
       </c>
     </row>
     <row r="12">
@@ -670,19 +670,19 @@
         <v>550000</v>
       </c>
       <c r="B12" t="n">
-        <v>43.4</v>
+        <v>40.2</v>
       </c>
       <c r="C12" t="n">
-        <v>34.55</v>
+        <v>29.9</v>
       </c>
       <c r="D12" t="n">
-        <v>76.05</v>
+        <v>88.55</v>
       </c>
       <c r="E12" t="n">
-        <v>509.25</v>
+        <v>499.25</v>
       </c>
       <c r="F12" t="n">
-        <v>374.7</v>
+        <v>356.05</v>
       </c>
     </row>
     <row r="13">
@@ -690,19 +690,19 @@
         <v>600000</v>
       </c>
       <c r="B13" t="n">
-        <v>48.3</v>
+        <v>42.45</v>
       </c>
       <c r="C13" t="n">
-        <v>37.15</v>
+        <v>33</v>
       </c>
       <c r="D13" t="n">
-        <v>82.59999999999999</v>
+        <v>99.09999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>561.9</v>
+        <v>558.7</v>
       </c>
       <c r="F13" t="n">
-        <v>407.75</v>
+        <v>390.75</v>
       </c>
     </row>
     <row r="14">
@@ -710,19 +710,19 @@
         <v>650000</v>
       </c>
       <c r="B14" t="n">
-        <v>52.6</v>
+        <v>47.7</v>
       </c>
       <c r="C14" t="n">
-        <v>39</v>
+        <v>33.9</v>
       </c>
       <c r="D14" t="n">
-        <v>90.2</v>
+        <v>115.05</v>
       </c>
       <c r="E14" t="n">
-        <v>614.1</v>
+        <v>604.75</v>
       </c>
       <c r="F14" t="n">
-        <v>445.25</v>
+        <v>424.8</v>
       </c>
     </row>
     <row r="15">
@@ -730,19 +730,19 @@
         <v>700000</v>
       </c>
       <c r="B15" t="n">
-        <v>57.45</v>
+        <v>52.1</v>
       </c>
       <c r="C15" t="n">
-        <v>42.2</v>
+        <v>37</v>
       </c>
       <c r="D15" t="n">
-        <v>95.09999999999999</v>
+        <v>123.9</v>
       </c>
       <c r="E15" t="n">
-        <v>660.55</v>
+        <v>647.9</v>
       </c>
       <c r="F15" t="n">
-        <v>482.2</v>
+        <v>460.45</v>
       </c>
     </row>
     <row r="16">
@@ -750,19 +750,19 @@
         <v>750000</v>
       </c>
       <c r="B16" t="n">
-        <v>63.9</v>
+        <v>60</v>
       </c>
       <c r="C16" t="n">
-        <v>44.95</v>
+        <v>40.6</v>
       </c>
       <c r="D16" t="n">
-        <v>100.9</v>
+        <v>135.05</v>
       </c>
       <c r="E16" t="n">
-        <v>705.05</v>
+        <v>708.85</v>
       </c>
       <c r="F16" t="n">
-        <v>520.15</v>
+        <v>502.25</v>
       </c>
     </row>
     <row r="17">
@@ -770,19 +770,19 @@
         <v>800000</v>
       </c>
       <c r="B17" t="n">
-        <v>66.8</v>
+        <v>63.65</v>
       </c>
       <c r="C17" t="n">
-        <v>47.5</v>
+        <v>43.1</v>
       </c>
       <c r="D17" t="n">
-        <v>109.3</v>
+        <v>143.5</v>
       </c>
       <c r="E17" t="n">
-        <v>749.2</v>
+        <v>753.5</v>
       </c>
       <c r="F17" t="n">
-        <v>558.2</v>
+        <v>536.7</v>
       </c>
     </row>
     <row r="18">
@@ -790,19 +790,19 @@
         <v>850000</v>
       </c>
       <c r="B18" t="n">
-        <v>70.8</v>
+        <v>65</v>
       </c>
       <c r="C18" t="n">
-        <v>51</v>
+        <v>44.4</v>
       </c>
       <c r="D18" t="n">
-        <v>115</v>
+        <v>148.65</v>
       </c>
       <c r="E18" t="n">
-        <v>792.05</v>
+        <v>784</v>
       </c>
       <c r="F18" t="n">
-        <v>596.35</v>
+        <v>570.15</v>
       </c>
     </row>
     <row r="19">
@@ -810,19 +810,19 @@
         <v>900000</v>
       </c>
       <c r="B19" t="n">
-        <v>73.2</v>
+        <v>66.75</v>
       </c>
       <c r="C19" t="n">
-        <v>52.15</v>
+        <v>45.85</v>
       </c>
       <c r="D19" t="n">
-        <v>120.6</v>
+        <v>155.65</v>
       </c>
       <c r="E19" t="n">
-        <v>827.45</v>
+        <v>820.45</v>
       </c>
       <c r="F19" t="n">
-        <v>629.25</v>
+        <v>599.7</v>
       </c>
     </row>
     <row r="20">
@@ -830,19 +830,19 @@
         <v>950000</v>
       </c>
       <c r="B20" t="n">
-        <v>76.25</v>
+        <v>69.7</v>
       </c>
       <c r="C20" t="n">
-        <v>58.65</v>
+        <v>51.95</v>
       </c>
       <c r="D20" t="n">
-        <v>127.4</v>
+        <v>164.55</v>
       </c>
       <c r="E20" t="n">
-        <v>869.7</v>
+        <v>864.25</v>
       </c>
       <c r="F20" t="n">
-        <v>669.6</v>
+        <v>638.75</v>
       </c>
     </row>
     <row r="21">
@@ -850,19 +850,19 @@
         <v>1000000</v>
       </c>
       <c r="B21" t="n">
-        <v>78.2</v>
+        <v>73.09999999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>64.34999999999999</v>
+        <v>59.3</v>
       </c>
       <c r="D21" t="n">
-        <v>134.1</v>
+        <v>173.2</v>
       </c>
       <c r="E21" t="n">
-        <v>913.55</v>
+        <v>904.65</v>
       </c>
       <c r="F21" t="n">
-        <v>708.9</v>
+        <v>676.5</v>
       </c>
     </row>
     <row r="22">
@@ -870,19 +870,19 @@
         <v>1050000</v>
       </c>
       <c r="B22" t="n">
-        <v>80.95</v>
+        <v>74.3</v>
       </c>
       <c r="C22" t="n">
-        <v>68.25</v>
+        <v>59.5</v>
       </c>
       <c r="D22" t="n">
-        <v>140.35</v>
+        <v>183.8</v>
       </c>
       <c r="E22" t="n">
-        <v>960.75</v>
+        <v>958.4</v>
       </c>
       <c r="F22" t="n">
-        <v>742.95</v>
+        <v>712.95</v>
       </c>
     </row>
     <row r="23">
@@ -890,19 +890,19 @@
         <v>1100000</v>
       </c>
       <c r="B23" t="n">
-        <v>88.7</v>
+        <v>81.05</v>
       </c>
       <c r="C23" t="n">
-        <v>70.59999999999999</v>
+        <v>63.6</v>
       </c>
       <c r="D23" t="n">
-        <v>156.05</v>
+        <v>189.4</v>
       </c>
       <c r="E23" t="n">
-        <v>1033.25</v>
+        <v>1031</v>
       </c>
       <c r="F23" t="n">
-        <v>782.6</v>
+        <v>750.65</v>
       </c>
     </row>
     <row r="24">
@@ -910,19 +910,19 @@
         <v>1150000</v>
       </c>
       <c r="B24" t="n">
-        <v>95.2</v>
+        <v>85.15000000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>74.25</v>
+        <v>65.34999999999999</v>
       </c>
       <c r="D24" t="n">
-        <v>169.3</v>
+        <v>196.9</v>
       </c>
       <c r="E24" t="n">
-        <v>1108.45</v>
+        <v>1092.7</v>
       </c>
       <c r="F24" t="n">
-        <v>826.9</v>
+        <v>790.35</v>
       </c>
     </row>
     <row r="25">
@@ -930,19 +930,19 @@
         <v>1200000</v>
       </c>
       <c r="B25" t="n">
-        <v>100.05</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>78.25</v>
+        <v>69</v>
       </c>
       <c r="D25" t="n">
-        <v>178.6</v>
+        <v>212.75</v>
       </c>
       <c r="E25" t="n">
-        <v>1177.75</v>
+        <v>1157.85</v>
       </c>
       <c r="F25" t="n">
-        <v>873.2</v>
+        <v>829.55</v>
       </c>
     </row>
     <row r="26">
@@ -950,19 +950,19 @@
         <v>1250000</v>
       </c>
       <c r="B26" t="n">
-        <v>102.5</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="C26" t="n">
-        <v>79.05</v>
+        <v>70.5</v>
       </c>
       <c r="D26" t="n">
-        <v>179.4</v>
+        <v>235.2</v>
       </c>
       <c r="E26" t="n">
-        <v>1191.45</v>
+        <v>1194.4</v>
       </c>
       <c r="F26" t="n">
-        <v>891.9</v>
+        <v>857.6</v>
       </c>
     </row>
     <row r="27">
@@ -970,19 +970,19 @@
         <v>1300000</v>
       </c>
       <c r="B27" t="n">
-        <v>107.7</v>
+        <v>99</v>
       </c>
       <c r="C27" t="n">
-        <v>80.75</v>
+        <v>71.95</v>
       </c>
       <c r="D27" t="n">
-        <v>188.7</v>
+        <v>244.1</v>
       </c>
       <c r="E27" t="n">
-        <v>1250.1</v>
+        <v>1244.15</v>
       </c>
       <c r="F27" t="n">
-        <v>934.4</v>
+        <v>897.2</v>
       </c>
     </row>
     <row r="28">
@@ -990,19 +990,19 @@
         <v>1350000</v>
       </c>
       <c r="B28" t="n">
-        <v>114.9</v>
+        <v>105.6</v>
       </c>
       <c r="C28" t="n">
-        <v>83.65000000000001</v>
+        <v>75.65000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>193.4</v>
+        <v>253.35</v>
       </c>
       <c r="E28" t="n">
-        <v>1293.1</v>
+        <v>1292.05</v>
       </c>
       <c r="F28" t="n">
-        <v>975.35</v>
+        <v>931.5</v>
       </c>
     </row>
     <row r="29">
@@ -1010,19 +1010,19 @@
         <v>1400000</v>
       </c>
       <c r="B29" t="n">
-        <v>119.95</v>
+        <v>111.75</v>
       </c>
       <c r="C29" t="n">
-        <v>87.55</v>
+        <v>78.7</v>
       </c>
       <c r="D29" t="n">
-        <v>199.95</v>
+        <v>261.8</v>
       </c>
       <c r="E29" t="n">
-        <v>1348.1</v>
+        <v>1343.1</v>
       </c>
       <c r="F29" t="n">
-        <v>1014.2</v>
+        <v>974.6</v>
       </c>
     </row>
     <row r="30">
@@ -1030,19 +1030,19 @@
         <v>1450000</v>
       </c>
       <c r="B30" t="n">
-        <v>122.7</v>
+        <v>115.5</v>
       </c>
       <c r="C30" t="n">
-        <v>89.34999999999999</v>
+        <v>82.2</v>
       </c>
       <c r="D30" t="n">
-        <v>205.3</v>
+        <v>274.5</v>
       </c>
       <c r="E30" t="n">
-        <v>1389.55</v>
+        <v>1396.1</v>
       </c>
       <c r="F30" t="n">
-        <v>1047.3</v>
+        <v>1016.5</v>
       </c>
     </row>
     <row r="31">
@@ -1050,19 +1050,19 @@
         <v>1500000</v>
       </c>
       <c r="B31" t="n">
-        <v>129.1</v>
+        <v>120.7</v>
       </c>
       <c r="C31" t="n">
-        <v>92.45</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>211.6</v>
+        <v>284.1</v>
       </c>
       <c r="E31" t="n">
-        <v>1432.8</v>
+        <v>1447.8</v>
       </c>
       <c r="F31" t="n">
-        <v>1085.2</v>
+        <v>1052.85</v>
       </c>
     </row>
     <row r="32">
@@ -1070,19 +1070,19 @@
         <v>1550000</v>
       </c>
       <c r="B32" t="n">
-        <v>133.15</v>
+        <v>126.4</v>
       </c>
       <c r="C32" t="n">
-        <v>96.05</v>
+        <v>86.8</v>
       </c>
       <c r="D32" t="n">
-        <v>219.95</v>
+        <v>290.35</v>
       </c>
       <c r="E32" t="n">
-        <v>1480.65</v>
+        <v>1492.65</v>
       </c>
       <c r="F32" t="n">
-        <v>1126.8</v>
+        <v>1091.95</v>
       </c>
     </row>
     <row r="33">
@@ -1090,19 +1090,19 @@
         <v>1600000</v>
       </c>
       <c r="B33" t="n">
-        <v>138.15</v>
+        <v>130.3</v>
       </c>
       <c r="C33" t="n">
-        <v>98.40000000000001</v>
+        <v>89.55</v>
       </c>
       <c r="D33" t="n">
-        <v>225.75</v>
+        <v>300.7</v>
       </c>
       <c r="E33" t="n">
-        <v>1519.5</v>
+        <v>1547.7</v>
       </c>
       <c r="F33" t="n">
-        <v>1161.1</v>
+        <v>1130.7</v>
       </c>
     </row>
     <row r="34">
@@ -1110,19 +1110,19 @@
         <v>1650000</v>
       </c>
       <c r="B34" t="n">
-        <v>144</v>
+        <v>134.35</v>
       </c>
       <c r="C34" t="n">
-        <v>101.25</v>
+        <v>91.65000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>234.75</v>
+        <v>309.45</v>
       </c>
       <c r="E34" t="n">
-        <v>1579.35</v>
+        <v>1571.85</v>
       </c>
       <c r="F34" t="n">
-        <v>1210.75</v>
+        <v>1167.45</v>
       </c>
     </row>
     <row r="35">
@@ -1130,19 +1130,19 @@
         <v>1700000</v>
       </c>
       <c r="B35" t="n">
-        <v>145.15</v>
+        <v>134.95</v>
       </c>
       <c r="C35" t="n">
-        <v>103.4</v>
+        <v>93.05</v>
       </c>
       <c r="D35" t="n">
-        <v>239.55</v>
+        <v>315.05</v>
       </c>
       <c r="E35" t="n">
-        <v>1610.75</v>
+        <v>1630.4</v>
       </c>
       <c r="F35" t="n">
-        <v>1243.8</v>
+        <v>1198.3</v>
       </c>
     </row>
     <row r="36">
@@ -1150,19 +1150,19 @@
         <v>1750000</v>
       </c>
       <c r="B36" t="n">
-        <v>150.35</v>
+        <v>139.25</v>
       </c>
       <c r="C36" t="n">
-        <v>107.6</v>
+        <v>96.05</v>
       </c>
       <c r="D36" t="n">
-        <v>246.85</v>
+        <v>326.2</v>
       </c>
       <c r="E36" t="n">
-        <v>1663.8</v>
+        <v>1661.65</v>
       </c>
       <c r="F36" t="n">
-        <v>1289.55</v>
+        <v>1243.25</v>
       </c>
     </row>
     <row r="37">
@@ -1170,19 +1170,19 @@
         <v>1800000</v>
       </c>
       <c r="B37" t="n">
-        <v>151.55</v>
+        <v>138.4</v>
       </c>
       <c r="C37" t="n">
-        <v>109.85</v>
+        <v>97.8</v>
       </c>
       <c r="D37" t="n">
-        <v>254.25</v>
+        <v>332.9</v>
       </c>
       <c r="E37" t="n">
-        <v>1697.3</v>
+        <v>1712.05</v>
       </c>
       <c r="F37" t="n">
-        <v>1326.3</v>
+        <v>1275.9</v>
       </c>
     </row>
     <row r="38">
@@ -1190,19 +1190,19 @@
         <v>1850000</v>
       </c>
       <c r="B38" t="n">
-        <v>156.8</v>
+        <v>143.65</v>
       </c>
       <c r="C38" t="n">
-        <v>115.75</v>
+        <v>103.1</v>
       </c>
       <c r="D38" t="n">
-        <v>263.8</v>
+        <v>347.2</v>
       </c>
       <c r="E38" t="n">
-        <v>1762.6</v>
+        <v>1765.5</v>
       </c>
       <c r="F38" t="n">
-        <v>1381.4</v>
+        <v>1315.8</v>
       </c>
     </row>
     <row r="39">
@@ -1210,19 +1210,19 @@
         <v>1900000</v>
       </c>
       <c r="B39" t="n">
-        <v>161.6</v>
+        <v>146.6</v>
       </c>
       <c r="C39" t="n">
-        <v>126.75</v>
+        <v>110.35</v>
       </c>
       <c r="D39" t="n">
-        <v>275.85</v>
+        <v>350.35</v>
       </c>
       <c r="E39" t="n">
-        <v>1818.6</v>
+        <v>1792.3</v>
       </c>
       <c r="F39" t="n">
-        <v>1434.15</v>
+        <v>1348.9</v>
       </c>
     </row>
     <row r="40">
@@ -1230,19 +1230,19 @@
         <v>1950000</v>
       </c>
       <c r="B40" t="n">
-        <v>164.45</v>
+        <v>147.85</v>
       </c>
       <c r="C40" t="n">
-        <v>135</v>
+        <v>117.25</v>
       </c>
       <c r="D40" t="n">
-        <v>277.9</v>
+        <v>358.2</v>
       </c>
       <c r="E40" t="n">
-        <v>1861.5</v>
+        <v>1814.95</v>
       </c>
       <c r="F40" t="n">
-        <v>1477.7</v>
+        <v>1380.35</v>
       </c>
     </row>
     <row r="41">
@@ -1250,19 +1250,19 @@
         <v>2000000</v>
       </c>
       <c r="B41" t="n">
-        <v>167</v>
+        <v>153.2</v>
       </c>
       <c r="C41" t="n">
-        <v>140.05</v>
+        <v>123.4</v>
       </c>
       <c r="D41" t="n">
-        <v>287.25</v>
+        <v>370.1</v>
       </c>
       <c r="E41" t="n">
-        <v>1907.3</v>
+        <v>1883.45</v>
       </c>
       <c r="F41" t="n">
-        <v>1514.2</v>
+        <v>1425.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>